<commit_message>
(#91)Added Tests for Basic Search Form
</commit_message>
<xml_diff>
--- a/test-data/cts_basic_search_functionality-data.xlsx
+++ b/test-data/cts_basic_search_functionality-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashkinaea/IdeaProjects/cgov-digital-platform-qa/test-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B067D3E3-C2C3-BE44-BEA2-851704EFD18F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A4E51B-69E1-4759-9980-185DBD935639}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30180" yWindow="5500" windowWidth="25600" windowHeight="14540" activeTab="2" xr2:uid="{02E62B52-A561-7E40-BFFB-9E993FCF680A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{02E62B52-A561-7E40-BFFB-9E993FCF680A}"/>
   </bookViews>
   <sheets>
     <sheet name="basic_search" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>path</t>
   </si>
@@ -166,13 +166,31 @@
   </si>
   <si>
     <t>WHICH TRIALS ARE RIGHT FOR YOU?</t>
+  </si>
+  <si>
+    <t>ExpectedPlaceholderText</t>
+  </si>
+  <si>
+    <t>Start typing to select a cancer type or keyword</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>crab</t>
+  </si>
+  <si>
+    <t>frye</t>
+  </si>
+  <si>
+    <t>No available options found. Your search will be based on the text above.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +201,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -209,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -219,6 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,21 +560,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BCB40F-6965-4647-B9F4-0250EB72F8C6}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.5" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="44.375" customWidth="1"/>
+    <col min="5" max="5" width="29.625" customWidth="1"/>
+    <col min="6" max="6" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -569,8 +596,11 @@
       <c r="G1" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -592,8 +622,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -615,8 +648,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -638,8 +674,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -661,8 +700,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -684,8 +726,11 @@
       <c r="G6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -706,6 +751,9 @@
       </c>
       <c r="G7" t="s">
         <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -716,21 +764,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6ACDCA-BBCE-6845-9351-00F3A72EB0AA}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" customWidth="1"/>
+    <col min="1" max="1" width="41.625" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
     <col min="5" max="5" width="35.5" customWidth="1"/>
+    <col min="7" max="7" width="61.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,8 +795,14 @@
       <c r="E1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -763,8 +818,14 @@
       <c r="E2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -780,8 +841,14 @@
       <c r="E3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -796,6 +863,12 @@
       </c>
       <c r="E4" t="s">
         <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -808,19 +881,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D25B56-660D-484F-847A-5F8835FDBCFC}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="43.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" customWidth="1"/>
-    <col min="5" max="6" width="46.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="1" max="2" width="43.375" customWidth="1"/>
+    <col min="4" max="4" width="23.875" customWidth="1"/>
+    <col min="5" max="6" width="46.875" customWidth="1"/>
+    <col min="7" max="7" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -843,7 +916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>

</xml_diff>